<commit_message>
Fixed the info in the XLSX for the Boss Stats. Then, fixed the CSV for that data. Created the import for the BossStats.csv.
</commit_message>
<xml_diff>
--- a/Data/World of Final Fantasy infodump.xlsx
+++ b/Data/World of Final Fantasy infodump.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="565">
   <si>
     <t>Adamantoise</t>
   </si>
@@ -1734,12 +1734,6 @@
   </si>
   <si>
     <t>Diabolos 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">		_x000D_
-Leviathan	68640	50	50	-150	0	150	0	-50	-50	100	100	100	100	100	100	100	100	75600	2360	Water Spellstone_x000D_
-Kyubi	23890	0	0	0	0	0	0	0	0	100	100	100	25	100	100	100	100	75600	2360	Mega Phoenix x1_x000D_
-Segwarides	25720	0	0	0	0	0	0	-50	50	100	100	100	100	100	100	100	100			</t>
   </si>
   <si>
     <t>Mega Phoenix x1</t>
@@ -2099,13 +2093,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2372,6 +2366,60 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FA67338-EDB5-428A-8BBB-6554102CB9E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9534525"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB5D98C-888D-4798-85C8-B3954D968DF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17533,7 +17581,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -21345,9 +21393,7 @@
       <c r="R62" s="62">
         <v>100</v>
       </c>
-      <c r="S62" s="89" t="s">
-        <v>563</v>
-      </c>
+      <c r="S62" s="87"/>
       <c r="T62" s="48"/>
       <c r="U62" s="48"/>
       <c r="V62" s="44"/>
@@ -21480,13 +21526,13 @@
         <v>2360</v>
       </c>
       <c r="U64" s="48" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="V64" s="44"/>
     </row>
     <row r="65" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B65" s="67">
         <v>25720</v>
@@ -45459,12 +45505,12 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="87" t="s">
+      <c r="A51" s="88" t="s">
         <v>548</v>
       </c>
-      <c r="B51" s="88"/>
-      <c r="C51" s="88"/>
-      <c r="D51" s="88"/>
+      <c r="B51" s="89"/>
+      <c r="C51" s="89"/>
+      <c r="D51" s="89"/>
       <c r="F51" s="83">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
Modified Resistances info. Got ResistanceItem import working. This was the last import. Next, we can start collating and converting the data.
</commit_message>
<xml_diff>
--- a/Data/World of Final Fantasy infodump.xlsx
+++ b/Data/World of Final Fantasy infodump.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Resistances" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
+            <family val="2"/>
           </rPr>
           <t>Source: SoulEaterTed - GameFAQs : https://www.gamefaqs.com/boards/168651-world-of-final-fantasy/74503708</t>
         </r>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="564">
   <si>
     <t>Adamantoise</t>
   </si>
@@ -1397,9 +1398,6 @@
     <t>#16 - Occult Fan 4</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>#17 Girls Diary 5</t>
   </si>
   <si>
@@ -1692,9 +1690,6 @@
   </si>
   <si>
     <t>---------------------</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>Glow Moogle</t>
@@ -1759,21 +1754,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2105,11 +2104,11 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2573,6 +2572,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{558B32F6-019D-4ABC-8674-348622214E50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9534525"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F00B1BFD-1D58-4300-B112-977918CD359D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9534525"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2875,8 +2982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A182" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
@@ -2945,10 +3052,10 @@
         <v>328</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="U1" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -3003,11 +3110,9 @@
       <c r="Q2" s="30">
         <v>50</v>
       </c>
-      <c r="R2" s="49" t="s">
-        <v>450</v>
-      </c>
+      <c r="R2" s="49"/>
       <c r="S2" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -3066,7 +3171,7 @@
         <v>4</v>
       </c>
       <c r="S3" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -3125,7 +3230,7 @@
         <v>5</v>
       </c>
       <c r="S4" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
@@ -3184,7 +3289,7 @@
         <v>7</v>
       </c>
       <c r="S5" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -3243,7 +3348,7 @@
         <v>2</v>
       </c>
       <c r="S6" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -3302,7 +3407,7 @@
         <v>2</v>
       </c>
       <c r="S7" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -3361,7 +3466,7 @@
         <v>2</v>
       </c>
       <c r="S8" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -3420,7 +3525,7 @@
         <v>5</v>
       </c>
       <c r="S9" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -3475,14 +3580,12 @@
       <c r="Q10" s="30">
         <v>25</v>
       </c>
-      <c r="R10" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R10" s="23"/>
       <c r="S10" s="24" t="s">
-        <v>472</v>
-      </c>
-      <c r="U10" t="s">
-        <v>549</v>
+        <v>471</v>
+      </c>
+      <c r="U10" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -3537,11 +3640,9 @@
       <c r="Q11" s="30">
         <v>25</v>
       </c>
-      <c r="R11" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R11" s="23"/>
       <c r="S11" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -3600,7 +3701,7 @@
         <v>7</v>
       </c>
       <c r="S12" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -3659,7 +3760,7 @@
         <v>5</v>
       </c>
       <c r="S13" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -3714,11 +3815,9 @@
       <c r="Q14" s="30">
         <v>50</v>
       </c>
-      <c r="R14" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R14" s="23"/>
       <c r="S14" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -3777,7 +3876,7 @@
         <v>1</v>
       </c>
       <c r="S15" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -3836,7 +3935,7 @@
         <v>3</v>
       </c>
       <c r="S16" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -3895,7 +3994,7 @@
         <v>3</v>
       </c>
       <c r="S17" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -3954,7 +4053,7 @@
         <v>4</v>
       </c>
       <c r="S18" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -4013,7 +4112,7 @@
         <v>3</v>
       </c>
       <c r="S19" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -4072,7 +4171,7 @@
         <v>5</v>
       </c>
       <c r="S20" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -4131,7 +4230,7 @@
         <v>1</v>
       </c>
       <c r="S21" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -4190,7 +4289,7 @@
         <v>5</v>
       </c>
       <c r="S22" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -4249,7 +4348,7 @@
         <v>1</v>
       </c>
       <c r="S23" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -4308,7 +4407,7 @@
         <v>1</v>
       </c>
       <c r="S24" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -4367,7 +4466,7 @@
         <v>5</v>
       </c>
       <c r="S25" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -4426,7 +4525,7 @@
         <v>6</v>
       </c>
       <c r="S26" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -4481,11 +4580,9 @@
       <c r="Q27" s="30">
         <v>50</v>
       </c>
-      <c r="R27" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R27" s="23"/>
       <c r="S27" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -4544,7 +4641,7 @@
         <v>3</v>
       </c>
       <c r="S28" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -4603,7 +4700,7 @@
         <v>1</v>
       </c>
       <c r="S29" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -4662,7 +4759,7 @@
         <v>7</v>
       </c>
       <c r="S30" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -4721,7 +4818,7 @@
         <v>3</v>
       </c>
       <c r="S31" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -4780,7 +4877,7 @@
         <v>3</v>
       </c>
       <c r="S32" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.25">
@@ -4839,7 +4936,7 @@
         <v>5</v>
       </c>
       <c r="S33" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
@@ -4898,7 +4995,7 @@
         <v>7</v>
       </c>
       <c r="S34" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.25">
@@ -4957,7 +5054,7 @@
         <v>2</v>
       </c>
       <c r="S35" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.25">
@@ -5016,7 +5113,7 @@
         <v>3</v>
       </c>
       <c r="S36" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.25">
@@ -5075,7 +5172,7 @@
         <v>4</v>
       </c>
       <c r="S37" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
@@ -5130,11 +5227,9 @@
       <c r="Q38" s="30">
         <v>50</v>
       </c>
-      <c r="R38" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R38" s="23"/>
       <c r="S38" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
@@ -5189,14 +5284,12 @@
       <c r="Q39" s="30">
         <v>50</v>
       </c>
-      <c r="R39" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R39" s="23"/>
       <c r="S39" s="24" t="s">
-        <v>472</v>
-      </c>
-      <c r="U39" t="s">
-        <v>549</v>
+        <v>471</v>
+      </c>
+      <c r="U39" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
@@ -5255,7 +5348,7 @@
         <v>5</v>
       </c>
       <c r="S40" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
@@ -5314,7 +5407,7 @@
         <v>5</v>
       </c>
       <c r="S41" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
@@ -5373,7 +5466,7 @@
         <v>5</v>
       </c>
       <c r="S42" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
@@ -5432,7 +5525,7 @@
         <v>7</v>
       </c>
       <c r="S43" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
@@ -5491,7 +5584,7 @@
         <v>6</v>
       </c>
       <c r="S44" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
@@ -5550,7 +5643,7 @@
         <v>6</v>
       </c>
       <c r="S45" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
@@ -5609,7 +5702,7 @@
         <v>3</v>
       </c>
       <c r="S46" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
@@ -5668,7 +5761,7 @@
         <v>6</v>
       </c>
       <c r="S47" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
@@ -5727,7 +5820,7 @@
         <v>6</v>
       </c>
       <c r="S48" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
@@ -5786,7 +5879,7 @@
         <v>3</v>
       </c>
       <c r="S49" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
@@ -5845,7 +5938,7 @@
         <v>5</v>
       </c>
       <c r="S50" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
@@ -5904,7 +5997,7 @@
         <v>5</v>
       </c>
       <c r="S51" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="52" spans="1:20" x14ac:dyDescent="0.25">
@@ -5963,7 +6056,7 @@
         <v>3</v>
       </c>
       <c r="S52" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
@@ -6022,7 +6115,7 @@
         <v>2</v>
       </c>
       <c r="S53" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
@@ -6081,7 +6174,7 @@
         <v>1</v>
       </c>
       <c r="S54" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
@@ -6140,7 +6233,7 @@
         <v>7</v>
       </c>
       <c r="S55" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
@@ -6199,7 +6292,7 @@
         <v>5</v>
       </c>
       <c r="S56" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
@@ -6258,7 +6351,7 @@
         <v>5</v>
       </c>
       <c r="S57" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
@@ -6317,7 +6410,7 @@
         <v>4</v>
       </c>
       <c r="S58" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
@@ -6376,7 +6469,7 @@
         <v>3</v>
       </c>
       <c r="S59" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
@@ -6435,12 +6528,12 @@
         <v>5</v>
       </c>
       <c r="S60" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="15" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B61" s="63">
         <v>0</v>
@@ -6494,10 +6587,10 @@
         <v>1</v>
       </c>
       <c r="S61" s="82" t="s">
-        <v>495</v>
-      </c>
-      <c r="T61" t="s">
-        <v>549</v>
+        <v>494</v>
+      </c>
+      <c r="T61" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
@@ -6556,7 +6649,7 @@
         <v>4</v>
       </c>
       <c r="S62" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
@@ -6615,7 +6708,7 @@
         <v>5</v>
       </c>
       <c r="S63" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
@@ -6674,7 +6767,7 @@
         <v>3</v>
       </c>
       <c r="S64" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.25">
@@ -6733,7 +6826,7 @@
         <v>7</v>
       </c>
       <c r="S65" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.25">
@@ -6792,7 +6885,7 @@
         <v>3</v>
       </c>
       <c r="S66" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.25">
@@ -6851,7 +6944,7 @@
         <v>1</v>
       </c>
       <c r="S67" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.25">
@@ -6910,7 +7003,7 @@
         <v>5</v>
       </c>
       <c r="S68" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -6969,10 +7062,10 @@
         <v>5</v>
       </c>
       <c r="S69" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U69" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U69" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.25">
@@ -7031,7 +7124,7 @@
         <v>6</v>
       </c>
       <c r="S70" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.25">
@@ -7090,10 +7183,10 @@
         <v>6</v>
       </c>
       <c r="S71" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U71" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U71" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.25">
@@ -7152,7 +7245,7 @@
         <v>1</v>
       </c>
       <c r="S72" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.25">
@@ -7207,11 +7300,9 @@
       <c r="Q73" s="30">
         <v>50</v>
       </c>
-      <c r="R73" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R73" s="23"/>
       <c r="S73" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.25">
@@ -7270,7 +7361,7 @@
         <v>7</v>
       </c>
       <c r="S74" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.25">
@@ -7329,7 +7420,7 @@
         <v>1</v>
       </c>
       <c r="S75" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.25">
@@ -7388,7 +7479,7 @@
         <v>6</v>
       </c>
       <c r="S76" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.25">
@@ -7447,7 +7538,7 @@
         <v>2</v>
       </c>
       <c r="S77" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.25">
@@ -7506,7 +7597,7 @@
         <v>6</v>
       </c>
       <c r="S78" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.25">
@@ -7565,7 +7656,7 @@
         <v>1</v>
       </c>
       <c r="S79" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
@@ -7624,7 +7715,7 @@
         <v>1</v>
       </c>
       <c r="S80" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.25">
@@ -7683,7 +7774,7 @@
         <v>7</v>
       </c>
       <c r="S81" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.25">
@@ -7742,7 +7833,7 @@
         <v>5</v>
       </c>
       <c r="S82" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.25">
@@ -7801,7 +7892,7 @@
         <v>6</v>
       </c>
       <c r="S83" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="T83" s="3"/>
     </row>
@@ -7861,7 +7952,7 @@
         <v>5</v>
       </c>
       <c r="S84" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.25">
@@ -7920,7 +8011,7 @@
         <v>6</v>
       </c>
       <c r="S85" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.25">
@@ -7975,11 +8066,9 @@
       <c r="Q86" s="30">
         <v>50</v>
       </c>
-      <c r="R86" s="49" t="s">
-        <v>450</v>
-      </c>
+      <c r="R86" s="49"/>
       <c r="S86" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.25">
@@ -8034,14 +8123,12 @@
       <c r="Q87" s="30">
         <v>25</v>
       </c>
-      <c r="R87" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R87" s="23"/>
       <c r="S87" s="24" t="s">
-        <v>472</v>
-      </c>
-      <c r="U87" t="s">
-        <v>549</v>
+        <v>471</v>
+      </c>
+      <c r="U87" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.25">
@@ -8100,7 +8187,7 @@
         <v>3</v>
       </c>
       <c r="S88" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.25">
@@ -8159,7 +8246,7 @@
         <v>6</v>
       </c>
       <c r="S89" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.25">
@@ -8218,7 +8305,7 @@
         <v>1</v>
       </c>
       <c r="S90" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.25">
@@ -8277,7 +8364,7 @@
         <v>1</v>
       </c>
       <c r="S91" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.25">
@@ -8336,7 +8423,7 @@
         <v>6</v>
       </c>
       <c r="S92" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.25">
@@ -8395,12 +8482,12 @@
         <v>6</v>
       </c>
       <c r="S93" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="B94" s="26">
         <v>25</v>
@@ -8454,10 +8541,10 @@
         <v>6</v>
       </c>
       <c r="S94" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="T94" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="T94" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.25">
@@ -8516,7 +8603,7 @@
         <v>6</v>
       </c>
       <c r="S95" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.25">
@@ -8575,7 +8662,7 @@
         <v>6</v>
       </c>
       <c r="S96" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.25">
@@ -8634,7 +8721,7 @@
         <v>6</v>
       </c>
       <c r="S97" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
@@ -8693,7 +8780,7 @@
         <v>6</v>
       </c>
       <c r="S98" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.25">
@@ -8752,7 +8839,7 @@
         <v>6</v>
       </c>
       <c r="S99" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.25">
@@ -8811,7 +8898,7 @@
         <v>2</v>
       </c>
       <c r="S100" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.25">
@@ -8870,7 +8957,7 @@
         <v>3</v>
       </c>
       <c r="S101" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.25">
@@ -8929,7 +9016,7 @@
         <v>1</v>
       </c>
       <c r="S102" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.25">
@@ -8988,7 +9075,7 @@
         <v>1</v>
       </c>
       <c r="S103" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
@@ -9047,7 +9134,7 @@
         <v>4</v>
       </c>
       <c r="S104" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.25">
@@ -9106,7 +9193,7 @@
         <v>5</v>
       </c>
       <c r="S105" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.25">
@@ -9165,10 +9252,10 @@
         <v>5</v>
       </c>
       <c r="S106" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U106" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U106" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.25">
@@ -9227,7 +9314,7 @@
         <v>7</v>
       </c>
       <c r="S107" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.25">
@@ -9286,7 +9373,7 @@
         <v>7</v>
       </c>
       <c r="S108" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.25">
@@ -9345,7 +9432,7 @@
         <v>7</v>
       </c>
       <c r="S109" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
@@ -9404,7 +9491,7 @@
         <v>5</v>
       </c>
       <c r="S110" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
@@ -9463,7 +9550,7 @@
         <v>5</v>
       </c>
       <c r="S111" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.25">
@@ -9522,7 +9609,7 @@
         <v>5</v>
       </c>
       <c r="S112" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="113" spans="1:20" x14ac:dyDescent="0.25">
@@ -9581,7 +9668,7 @@
         <v>6</v>
       </c>
       <c r="S113" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="114" spans="1:20" x14ac:dyDescent="0.25">
@@ -9640,12 +9727,12 @@
         <v>4</v>
       </c>
       <c r="S114" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="15" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B115" s="26">
         <v>0</v>
@@ -9699,10 +9786,10 @@
         <v>2</v>
       </c>
       <c r="S115" s="24" t="s">
-        <v>495</v>
-      </c>
-      <c r="T115" t="s">
-        <v>549</v>
+        <v>494</v>
+      </c>
+      <c r="T115" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="116" spans="1:20" x14ac:dyDescent="0.25">
@@ -9761,7 +9848,7 @@
         <v>3</v>
       </c>
       <c r="S116" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="117" spans="1:20" x14ac:dyDescent="0.25">
@@ -9820,7 +9907,7 @@
         <v>3</v>
       </c>
       <c r="S117" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="118" spans="1:20" x14ac:dyDescent="0.25">
@@ -9879,7 +9966,7 @@
         <v>3</v>
       </c>
       <c r="S118" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="119" spans="1:20" x14ac:dyDescent="0.25">
@@ -9938,7 +10025,7 @@
         <v>7</v>
       </c>
       <c r="S119" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="120" spans="1:20" x14ac:dyDescent="0.25">
@@ -9997,7 +10084,7 @@
         <v>4</v>
       </c>
       <c r="S120" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="121" spans="1:20" x14ac:dyDescent="0.25">
@@ -10056,12 +10143,12 @@
         <v>3</v>
       </c>
       <c r="S121" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B122" s="26">
         <v>0</v>
@@ -10115,10 +10202,10 @@
         <v>2</v>
       </c>
       <c r="S122" s="24" t="s">
-        <v>495</v>
-      </c>
-      <c r="T122" t="s">
-        <v>549</v>
+        <v>494</v>
+      </c>
+      <c r="T122" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="123" spans="1:20" x14ac:dyDescent="0.25">
@@ -10177,7 +10264,7 @@
         <v>1</v>
       </c>
       <c r="S123" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="124" spans="1:20" x14ac:dyDescent="0.25">
@@ -10236,7 +10323,7 @@
         <v>3</v>
       </c>
       <c r="S124" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="125" spans="1:20" x14ac:dyDescent="0.25">
@@ -10295,7 +10382,7 @@
         <v>3</v>
       </c>
       <c r="S125" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="126" spans="1:20" x14ac:dyDescent="0.25">
@@ -10354,7 +10441,7 @@
         <v>7</v>
       </c>
       <c r="S126" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="127" spans="1:20" x14ac:dyDescent="0.25">
@@ -10413,7 +10500,7 @@
         <v>5</v>
       </c>
       <c r="S127" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="128" spans="1:20" x14ac:dyDescent="0.25">
@@ -10472,7 +10559,7 @@
         <v>4</v>
       </c>
       <c r="S128" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="129" spans="1:21" x14ac:dyDescent="0.25">
@@ -10531,7 +10618,7 @@
         <v>5</v>
       </c>
       <c r="S129" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="130" spans="1:21" x14ac:dyDescent="0.25">
@@ -10590,7 +10677,7 @@
         <v>5</v>
       </c>
       <c r="S130" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="131" spans="1:21" x14ac:dyDescent="0.25">
@@ -10645,11 +10732,9 @@
       <c r="Q131" s="30">
         <v>50</v>
       </c>
-      <c r="R131" s="49" t="s">
-        <v>450</v>
-      </c>
+      <c r="R131" s="49"/>
       <c r="S131" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.25">
@@ -10704,14 +10789,12 @@
       <c r="Q132" s="30">
         <v>50</v>
       </c>
-      <c r="R132" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R132" s="23"/>
       <c r="S132" s="24" t="s">
-        <v>472</v>
-      </c>
-      <c r="U132" t="s">
-        <v>549</v>
+        <v>471</v>
+      </c>
+      <c r="U132" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
@@ -10770,7 +10853,7 @@
         <v>7</v>
       </c>
       <c r="S133" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="134" spans="1:21" x14ac:dyDescent="0.25">
@@ -10829,12 +10912,12 @@
         <v>7</v>
       </c>
       <c r="S134" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A135" s="15" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B135" s="26">
         <v>25</v>
@@ -10884,14 +10967,12 @@
       <c r="Q135" s="30">
         <v>25</v>
       </c>
-      <c r="R135" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R135" s="23"/>
       <c r="S135" s="24" t="s">
-        <v>472</v>
-      </c>
-      <c r="T135" t="s">
-        <v>549</v>
+        <v>471</v>
+      </c>
+      <c r="T135" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="136" spans="1:21" x14ac:dyDescent="0.25">
@@ -10950,7 +11031,7 @@
         <v>4</v>
       </c>
       <c r="S136" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="137" spans="1:21" x14ac:dyDescent="0.25">
@@ -11009,7 +11090,7 @@
         <v>6</v>
       </c>
       <c r="S137" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="138" spans="1:21" x14ac:dyDescent="0.25">
@@ -11068,7 +11149,7 @@
         <v>5</v>
       </c>
       <c r="S138" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="139" spans="1:21" x14ac:dyDescent="0.25">
@@ -11127,7 +11208,7 @@
         <v>4</v>
       </c>
       <c r="S139" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.25">
@@ -11186,10 +11267,10 @@
         <v>4</v>
       </c>
       <c r="S140" s="24" t="s">
-        <v>490</v>
-      </c>
-      <c r="U140" t="s">
-        <v>549</v>
+        <v>489</v>
+      </c>
+      <c r="U140" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.25">
@@ -11248,7 +11329,7 @@
         <v>2</v>
       </c>
       <c r="S141" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.25">
@@ -11307,7 +11388,7 @@
         <v>2</v>
       </c>
       <c r="S142" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.25">
@@ -11366,7 +11447,7 @@
         <v>5</v>
       </c>
       <c r="S143" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
@@ -11425,10 +11506,10 @@
         <v>5</v>
       </c>
       <c r="S144" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U144" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U144" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="145" spans="1:21" x14ac:dyDescent="0.25">
@@ -11487,7 +11568,7 @@
         <v>5</v>
       </c>
       <c r="S145" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="146" spans="1:21" x14ac:dyDescent="0.25">
@@ -11546,7 +11627,7 @@
         <v>7</v>
       </c>
       <c r="S146" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.25">
@@ -11605,10 +11686,10 @@
         <v>7</v>
       </c>
       <c r="S147" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U147" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U147" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.25">
@@ -11667,7 +11748,7 @@
         <v>6</v>
       </c>
       <c r="S148" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="149" spans="1:21" x14ac:dyDescent="0.25">
@@ -11726,10 +11807,10 @@
         <v>6</v>
       </c>
       <c r="S149" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U149" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U149" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="150" spans="1:21" x14ac:dyDescent="0.25">
@@ -11788,12 +11869,12 @@
         <v>3</v>
       </c>
       <c r="S150" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151" s="15" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="B151" s="26">
         <v>25</v>
@@ -11847,10 +11928,10 @@
         <v>2</v>
       </c>
       <c r="S151" s="24" t="s">
-        <v>495</v>
-      </c>
-      <c r="T151" t="s">
-        <v>549</v>
+        <v>494</v>
+      </c>
+      <c r="T151" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="152" spans="1:21" x14ac:dyDescent="0.25">
@@ -11909,7 +11990,7 @@
         <v>4</v>
       </c>
       <c r="S152" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="153" spans="1:21" x14ac:dyDescent="0.25">
@@ -11968,7 +12049,7 @@
         <v>4</v>
       </c>
       <c r="S153" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.25">
@@ -12027,7 +12108,7 @@
         <v>6</v>
       </c>
       <c r="S154" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.25">
@@ -12086,7 +12167,7 @@
         <v>6</v>
       </c>
       <c r="S155" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.25">
@@ -12145,7 +12226,7 @@
         <v>7</v>
       </c>
       <c r="S156" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.25">
@@ -12204,7 +12285,7 @@
         <v>3</v>
       </c>
       <c r="S157" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.25">
@@ -12263,7 +12344,7 @@
         <v>4</v>
       </c>
       <c r="S158" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="159" spans="1:21" x14ac:dyDescent="0.25">
@@ -12322,7 +12403,7 @@
         <v>4</v>
       </c>
       <c r="S159" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="160" spans="1:21" x14ac:dyDescent="0.25">
@@ -12381,7 +12462,7 @@
         <v>7</v>
       </c>
       <c r="S160" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.25">
@@ -12440,7 +12521,7 @@
         <v>2</v>
       </c>
       <c r="S161" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.25">
@@ -12499,7 +12580,7 @@
         <v>2</v>
       </c>
       <c r="S162" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="163" spans="1:21" x14ac:dyDescent="0.25">
@@ -12558,7 +12639,7 @@
         <v>2</v>
       </c>
       <c r="S163" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="164" spans="1:21" x14ac:dyDescent="0.25">
@@ -12617,7 +12698,7 @@
         <v>4</v>
       </c>
       <c r="S164" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="165" spans="1:21" x14ac:dyDescent="0.25">
@@ -12676,7 +12757,7 @@
         <v>5</v>
       </c>
       <c r="S165" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="166" spans="1:21" x14ac:dyDescent="0.25">
@@ -12735,10 +12816,10 @@
         <v>5</v>
       </c>
       <c r="S166" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U166" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U166" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="167" spans="1:21" x14ac:dyDescent="0.25">
@@ -12797,7 +12878,7 @@
         <v>5</v>
       </c>
       <c r="S167" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.25">
@@ -12856,10 +12937,10 @@
         <v>5</v>
       </c>
       <c r="S168" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U168" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U168" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.25">
@@ -12918,7 +12999,7 @@
         <v>5</v>
       </c>
       <c r="S169" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.25">
@@ -12977,7 +13058,7 @@
         <v>3</v>
       </c>
       <c r="S170" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.25">
@@ -13036,7 +13117,7 @@
         <v>5</v>
       </c>
       <c r="S171" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.25">
@@ -13095,7 +13176,7 @@
         <v>5</v>
       </c>
       <c r="S172" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.25">
@@ -13154,7 +13235,7 @@
         <v>5</v>
       </c>
       <c r="S173" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.25">
@@ -13213,7 +13294,7 @@
         <v>3</v>
       </c>
       <c r="S174" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.25">
@@ -13272,7 +13353,7 @@
         <v>7</v>
       </c>
       <c r="S175" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.25">
@@ -13331,7 +13412,7 @@
         <v>4</v>
       </c>
       <c r="S176" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="177" spans="1:21" x14ac:dyDescent="0.25">
@@ -13390,7 +13471,7 @@
         <v>1</v>
       </c>
       <c r="S177" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="178" spans="1:21" x14ac:dyDescent="0.25">
@@ -13449,7 +13530,7 @@
         <v>2</v>
       </c>
       <c r="S178" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="179" spans="1:21" x14ac:dyDescent="0.25">
@@ -13508,7 +13589,7 @@
         <v>6</v>
       </c>
       <c r="S179" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="180" spans="1:21" x14ac:dyDescent="0.25">
@@ -13567,7 +13648,7 @@
         <v>7</v>
       </c>
       <c r="S180" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.25">
@@ -13626,7 +13707,7 @@
         <v>7</v>
       </c>
       <c r="S181" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.25">
@@ -13685,7 +13766,7 @@
         <v>4</v>
       </c>
       <c r="S182" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.25">
@@ -13744,7 +13825,7 @@
         <v>6</v>
       </c>
       <c r="S183" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.25">
@@ -13803,7 +13884,7 @@
         <v>7</v>
       </c>
       <c r="S184" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="185" spans="1:21" x14ac:dyDescent="0.25">
@@ -13858,11 +13939,9 @@
       <c r="Q185" s="30">
         <v>50</v>
       </c>
-      <c r="R185" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R185" s="23"/>
       <c r="S185" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="186" spans="1:21" x14ac:dyDescent="0.25">
@@ -13921,7 +14000,7 @@
         <v>7</v>
       </c>
       <c r="S186" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="187" spans="1:21" x14ac:dyDescent="0.25">
@@ -13980,10 +14059,10 @@
         <v>6</v>
       </c>
       <c r="S187" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U187" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U187" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.25">
@@ -14042,7 +14121,7 @@
         <v>5</v>
       </c>
       <c r="S188" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.25">
@@ -14101,10 +14180,10 @@
         <v>5</v>
       </c>
       <c r="S189" s="24" t="s">
-        <v>493</v>
-      </c>
-      <c r="U189" t="s">
-        <v>549</v>
+        <v>492</v>
+      </c>
+      <c r="U189" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="190" spans="1:21" x14ac:dyDescent="0.25">
@@ -14163,7 +14242,7 @@
         <v>5</v>
       </c>
       <c r="S190" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="191" spans="1:21" x14ac:dyDescent="0.25">
@@ -14222,7 +14301,7 @@
         <v>5</v>
       </c>
       <c r="S191" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.25">
@@ -14281,7 +14360,7 @@
         <v>4</v>
       </c>
       <c r="S192" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="193" spans="1:20" x14ac:dyDescent="0.25">
@@ -14340,7 +14419,7 @@
         <v>5</v>
       </c>
       <c r="S193" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="194" spans="1:20" x14ac:dyDescent="0.25">
@@ -14399,7 +14478,7 @@
         <v>3</v>
       </c>
       <c r="S194" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="195" spans="1:20" x14ac:dyDescent="0.25">
@@ -14458,7 +14537,7 @@
         <v>7</v>
       </c>
       <c r="S195" s="24" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="196" spans="1:20" x14ac:dyDescent="0.25">
@@ -14517,7 +14596,7 @@
         <v>3</v>
       </c>
       <c r="S196" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="197" spans="1:20" x14ac:dyDescent="0.25">
@@ -14576,7 +14655,7 @@
         <v>3</v>
       </c>
       <c r="S197" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="198" spans="1:20" x14ac:dyDescent="0.25">
@@ -14635,7 +14714,7 @@
         <v>1</v>
       </c>
       <c r="S198" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="199" spans="1:20" x14ac:dyDescent="0.25">
@@ -14694,12 +14773,12 @@
         <v>1</v>
       </c>
       <c r="S199" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200" s="15" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="B200" s="26">
         <v>-25</v>
@@ -14753,10 +14832,10 @@
         <v>3</v>
       </c>
       <c r="S200" s="24" t="s">
-        <v>490</v>
-      </c>
-      <c r="T200" t="s">
-        <v>549</v>
+        <v>489</v>
+      </c>
+      <c r="T200" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="201" spans="1:20" x14ac:dyDescent="0.25">
@@ -14815,7 +14894,7 @@
         <v>3</v>
       </c>
       <c r="S201" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="202" spans="1:20" x14ac:dyDescent="0.25">
@@ -14874,7 +14953,7 @@
         <v>3</v>
       </c>
       <c r="S202" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="203" spans="1:20" x14ac:dyDescent="0.25">
@@ -14929,11 +15008,9 @@
       <c r="Q203" s="30">
         <v>50</v>
       </c>
-      <c r="R203" s="23" t="s">
-        <v>450</v>
-      </c>
+      <c r="R203" s="23"/>
       <c r="S203" s="24" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.25">
@@ -14992,7 +15069,7 @@
         <v>2</v>
       </c>
       <c r="S204" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T204" s="3"/>
     </row>
@@ -15052,7 +15129,7 @@
         <v>4</v>
       </c>
       <c r="S205" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="206" spans="1:20" x14ac:dyDescent="0.25">
@@ -15111,7 +15188,7 @@
         <v>2</v>
       </c>
       <c r="S206" s="24" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.25">
@@ -15879,8 +15956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E186" sqref="E186"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15898,13 +15975,13 @@
         <v>205</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -15981,8 +16058,8 @@
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="90" t="s">
-        <v>565</v>
+      <c r="E10" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -16234,8 +16311,8 @@
       <c r="B39" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E39" s="90" t="s">
-        <v>565</v>
+      <c r="E39" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -16496,8 +16573,8 @@
       <c r="B68" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E68" s="90" t="s">
-        <v>565</v>
+      <c r="E68" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -16515,8 +16592,8 @@
       <c r="B70" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E70" s="90" t="s">
-        <v>565</v>
+      <c r="E70" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="71" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -16667,8 +16744,8 @@
       <c r="B86" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E86" s="90" t="s">
-        <v>565</v>
+      <c r="E86" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -16820,8 +16897,8 @@
       <c r="B104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="90" t="s">
-        <v>565</v>
+      <c r="E104" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -16893,13 +16970,13 @@
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="15" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B113" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D113" s="90" t="s">
-        <v>565</v>
+      <c r="D113" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -16952,13 +17029,13 @@
     </row>
     <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B120" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="D120" s="90" t="s">
-        <v>565</v>
+      <c r="D120" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -17044,8 +17121,8 @@
       <c r="B130" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E130" s="90" t="s">
-        <v>565</v>
+      <c r="E130" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17072,13 +17149,13 @@
     </row>
     <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="15" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B133" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D133" s="90" t="s">
-        <v>565</v>
+      <c r="D133" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17126,8 +17203,8 @@
       <c r="B138" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E138" s="90" t="s">
-        <v>565</v>
+      <c r="E138" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17161,8 +17238,8 @@
       <c r="B142" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E142" s="90" t="s">
-        <v>565</v>
+      <c r="E142" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17188,8 +17265,8 @@
       <c r="B145" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E145" s="90" t="s">
-        <v>565</v>
+      <c r="E145" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17207,8 +17284,8 @@
       <c r="B147" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E147" s="90" t="s">
-        <v>565</v>
+      <c r="E147" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17338,8 +17415,8 @@
       <c r="B163" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E163" s="90" t="s">
-        <v>565</v>
+      <c r="E163" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="164" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17357,8 +17434,8 @@
       <c r="B165" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E165" s="90" t="s">
-        <v>565</v>
+      <c r="E165" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="166" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17521,8 +17598,8 @@
       <c r="B184" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="E184" s="90" t="s">
-        <v>565</v>
+      <c r="E184" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="185" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17540,8 +17617,8 @@
       <c r="B186" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="E186" s="90" t="s">
-        <v>565</v>
+      <c r="E186" s="88" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="187" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -17718,7 +17795,7 @@
         <v>204</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>3</v>
@@ -17769,7 +17846,7 @@
         <v>233</v>
       </c>
       <c r="S1" s="19" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="T1" s="19" t="s">
         <v>247</v>
@@ -17778,7 +17855,7 @@
         <v>250</v>
       </c>
       <c r="V1" s="20" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18470,12 +18547,12 @@
       <c r="T12" s="19"/>
       <c r="U12" s="19"/>
       <c r="V12" s="20" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B13" s="21">
         <v>2860</v>
@@ -18535,7 +18612,7 @@
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B14" s="21">
         <v>1350</v>
@@ -18652,12 +18729,12 @@
       <c r="T15" s="19"/>
       <c r="U15" s="19"/>
       <c r="V15" s="20" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B16" s="21">
         <v>3530</v>
@@ -18719,7 +18796,7 @@
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B17" s="21">
         <v>3840</v>
@@ -18777,7 +18854,7 @@
       </c>
       <c r="T17" s="19"/>
       <c r="U17" s="19" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="V17" s="44"/>
     </row>
@@ -18843,13 +18920,13 @@
         <v>7200</v>
       </c>
       <c r="U18" s="19" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="V18" s="44"/>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21">
@@ -18906,7 +18983,7 @@
       <c r="T19" s="19"/>
       <c r="U19" s="19"/>
       <c r="V19" s="20" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -18971,10 +19048,10 @@
         <v>1000</v>
       </c>
       <c r="U20" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="V20" s="20" t="s">
         <v>499</v>
-      </c>
-      <c r="V20" s="20" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19038,7 +19115,7 @@
       <c r="T21" s="19"/>
       <c r="U21" s="19"/>
       <c r="V21" s="20" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19102,12 +19179,12 @@
       <c r="T22" s="19"/>
       <c r="U22" s="19"/>
       <c r="V22" s="20" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B23" s="21">
         <v>9646</v>
@@ -19231,10 +19308,10 @@
       </c>
       <c r="T24" s="19"/>
       <c r="U24" s="19" t="s">
+        <v>507</v>
+      </c>
+      <c r="V24" s="20" t="s">
         <v>508</v>
-      </c>
-      <c r="V24" s="20" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19299,10 +19376,10 @@
         <v>1200</v>
       </c>
       <c r="U25" s="19" t="s">
+        <v>509</v>
+      </c>
+      <c r="V25" s="20" t="s">
         <v>510</v>
-      </c>
-      <c r="V25" s="20" t="s">
-        <v>511</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19368,12 +19445,12 @@
       </c>
       <c r="U26" s="19"/>
       <c r="V26" s="20" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B27" s="21">
         <v>10220</v>
@@ -19491,10 +19568,10 @@
       </c>
       <c r="T28" s="19"/>
       <c r="U28" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="V28" s="20" t="s">
         <v>514</v>
-      </c>
-      <c r="V28" s="20" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -19649,7 +19726,7 @@
     </row>
     <row r="32" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B32" s="21">
         <v>10050</v>
@@ -19706,12 +19783,12 @@
       <c r="T32" s="19"/>
       <c r="U32" s="19"/>
       <c r="V32" s="20" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B33" s="21">
         <v>2637</v>
@@ -19881,15 +19958,15 @@
         <v>2000</v>
       </c>
       <c r="U35" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="V35" s="20" t="s">
         <v>519</v>
-      </c>
-      <c r="V35" s="20" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="36" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -19979,7 +20056,7 @@
         <v>3000</v>
       </c>
       <c r="U37" s="19" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="V37" s="44"/>
     </row>
@@ -20045,13 +20122,13 @@
         <v>3962</v>
       </c>
       <c r="U38" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="V38" s="44"/>
     </row>
     <row r="39" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B39" s="21">
         <v>1349</v>
@@ -20095,7 +20172,7 @@
     </row>
     <row r="40" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B40" s="21">
         <v>1356</v>
@@ -20215,7 +20292,7 @@
         <v>4424</v>
       </c>
       <c r="U41" s="19" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="V41" s="44"/>
     </row>
@@ -20325,13 +20402,13 @@
         <v>3976</v>
       </c>
       <c r="U43" s="19" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="V43" s="44"/>
     </row>
     <row r="44" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B44" s="21">
         <v>14607</v>
@@ -20435,7 +20512,7 @@
         <v>412</v>
       </c>
       <c r="U45" s="19" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="V45" s="44"/>
     </row>
@@ -20561,7 +20638,7 @@
         <v>412</v>
       </c>
       <c r="U47" s="19" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="V47" s="44"/>
     </row>
@@ -20627,7 +20704,7 @@
     </row>
     <row r="49" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B49" s="21">
         <v>35036</v>
@@ -20687,13 +20764,13 @@
         <v>4320</v>
       </c>
       <c r="U49" s="19" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="V49" s="44"/>
     </row>
     <row r="50" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B50" s="21">
         <v>18810</v>
@@ -20753,13 +20830,13 @@
         <v>2260</v>
       </c>
       <c r="U50" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="V50" s="44"/>
     </row>
     <row r="51" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B51" s="21">
         <v>19610</v>
@@ -20819,13 +20896,13 @@
         <v>1425</v>
       </c>
       <c r="U51" s="19" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="V51" s="44"/>
     </row>
     <row r="52" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B52" s="21">
         <v>73820</v>
@@ -20885,7 +20962,7 @@
     </row>
     <row r="53" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B53" s="21">
         <v>13001</v>
@@ -21011,13 +21088,13 @@
         <v>540</v>
       </c>
       <c r="U54" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="V54" s="44"/>
     </row>
     <row r="55" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B55" s="21">
         <v>9480</v>
@@ -21077,13 +21154,13 @@
         <v>540</v>
       </c>
       <c r="U55" s="19" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="V55" s="44"/>
     </row>
     <row r="56" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B56" s="21">
         <v>23159</v>
@@ -21143,13 +21220,13 @@
         <v>5400</v>
       </c>
       <c r="U56" s="19" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="V56" s="44"/>
     </row>
     <row r="57" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B57" s="21">
         <v>22930</v>
@@ -21209,7 +21286,7 @@
     </row>
     <row r="58" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B58" s="21">
         <v>23610</v>
@@ -21329,13 +21406,13 @@
         <v>2360</v>
       </c>
       <c r="U59" s="19" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="V59" s="44"/>
     </row>
     <row r="60" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B60" s="21">
         <v>148000</v>
@@ -21455,13 +21532,13 @@
         <v>2360</v>
       </c>
       <c r="U61" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="V61" s="44"/>
     </row>
     <row r="62" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B62" s="67">
         <v>69170</v>
@@ -21581,7 +21658,7 @@
         <v>2360</v>
       </c>
       <c r="U63" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="V63" s="44"/>
     </row>
@@ -21647,13 +21724,13 @@
         <v>2360</v>
       </c>
       <c r="U64" s="48" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="V64" s="44"/>
     </row>
     <row r="65" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B65" s="67">
         <v>25720</v>
@@ -43919,97 +43996,97 @@
     </row>
     <row r="117" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="119" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="120" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="121" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="122" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="123" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="124" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="125" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="126" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="127" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="128" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="130" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="131" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="132" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="133" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="134" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="135" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="136" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="137" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="138" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
@@ -44019,12 +44096,12 @@
     </row>
     <row r="139" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="140" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="142" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
@@ -44034,72 +44111,72 @@
     </row>
     <row r="143" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="144" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="145" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="147" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="148" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="150" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="151" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="152" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="154" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="155" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="156" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="157" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="158" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="159" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
   </sheetData>
@@ -44131,29 +44208,29 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="51" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B1" s="51" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C1" s="51" t="s">
+        <v>505</v>
+      </c>
+      <c r="D1" s="51" t="s">
         <v>506</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>507</v>
       </c>
       <c r="E1" s="52"/>
       <c r="F1" s="51" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G1" s="51" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="H1" s="51" t="s">
+        <v>505</v>
+      </c>
+      <c r="I1" s="51" t="s">
         <v>506</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -45626,17 +45703,17 @@
       </c>
     </row>
     <row r="51" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="88" t="s">
-        <v>547</v>
-      </c>
-      <c r="B51" s="89"/>
-      <c r="C51" s="89"/>
-      <c r="D51" s="89"/>
+      <c r="A51" s="89" t="s">
+        <v>546</v>
+      </c>
+      <c r="B51" s="90"/>
+      <c r="C51" s="90"/>
+      <c r="D51" s="90"/>
       <c r="F51" s="83">
         <v>99</v>
       </c>
       <c r="G51" s="84" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="H51" s="84">
         <f t="shared" si="1"/>

</xml_diff>